<commit_message>
Mejoras código y comprobación de resultados.
</commit_message>
<xml_diff>
--- a/INPUT/Resultados/patogenicos_0.xlsx
+++ b/INPUT/Resultados/patogenicos_0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
   <si>
     <t>Número de chip</t>
   </si>
@@ -115,6 +115,9 @@
     <t>00028</t>
   </si>
   <si>
+    <t>1234567</t>
+  </si>
+  <si>
     <t>23B00021-A1</t>
   </si>
   <si>
@@ -139,7 +142,16 @@
     <t>23B00028-A2</t>
   </si>
   <si>
+    <t>23B000000-A1/CHIP100.1</t>
+  </si>
+  <si>
+    <t>23B00000-A1/CHIP100.2</t>
+  </si>
+  <si>
     <t>24-mar-2023</t>
+  </si>
+  <si>
+    <t>25-may-2023</t>
   </si>
   <si>
     <t>Carcinoma pulmonar no microcítico</t>
@@ -527,7 +539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -594,28 +606,28 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H2">
         <v>15.1</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -644,28 +656,28 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H3">
         <v>15.1</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -694,28 +706,28 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H4">
         <v>15.1</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -744,28 +756,28 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H5">
         <v>15.1</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -794,28 +806,28 @@
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H6">
         <v>15.1</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -844,28 +856,28 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H7">
         <v>15.1</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -894,28 +906,28 @@
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -944,42 +956,142 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H9">
         <v>11</v>
       </c>
       <c r="I9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="J9" t="s">
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10">
+        <v>15.1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
         <v>45</v>
       </c>
-      <c r="K9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11">
+        <v>15.1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
         <v>1</v>
       </c>
     </row>

</xml_diff>